<commit_message>
Added method for single line import of AGS CPT data
</commit_message>
<xml_diff>
--- a/notebooks/Data/excel_example.xlsx
+++ b/notebooks/Data/excel_example.xlsx
@@ -1,24 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profound/Documents/UGent/Geotechniek/Exercises/Exercise exam/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/profound/Documents/SourceTree.tmp/ProFound/groundhog/notebooks/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{388AA1CE-B14C-424C-8215-9E268AFF8E82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B368EC55-69CE-D642-8D69-42D809C0102F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{6FE22D12-2EFE-3D4F-B7D5-0238C04AC532}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -412,7 +420,7 @@
   <dimension ref="A1:E1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>